<commit_message>
Binek arac son eklemeler
</commit_message>
<xml_diff>
--- a/r_input/kredi_indirimi.xlsx
+++ b/r_input/kredi_indirimi.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\eski bilgisayarlar\ICCT harddisk\ICCT blgisayar\Turkey- Tax System\R\TR_tax_system\r_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8F1273-6722-472B-9EC4-BC2101953D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94AA8D9-7D3D-4114-970A-D1671B5A33B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F678959E-5C45-4896-80A4-1E09A95E6608}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F678959E-5C45-4896-80A4-1E09A95E6608}"/>
   </bookViews>
   <sheets>
     <sheet name="binek" sheetId="1" r:id="rId1"/>
     <sheet name="LCV" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>degisken</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>lcv_max indirimli kredi miktari</t>
+  </si>
+  <si>
+    <t>kredi_talep_esnekligi</t>
   </si>
 </sst>
 </file>
@@ -447,10 +450,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -496,7 +499,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -505,6 +508,14 @@
       </c>
       <c r="B6" s="3">
         <v>100000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.63</v>
       </c>
     </row>
   </sheetData>
@@ -517,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D26063-1C04-4862-9558-960AB0E64F44}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
kredi faiz indirimi yontemi degistirildi
</commit_message>
<xml_diff>
--- a/r_input/kredi_indirimi.xlsx
+++ b/r_input/kredi_indirimi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\eski bilgisayarlar\ICCT harddisk\ICCT blgisayar\Turkey- Tax System\R\TR_tax_system\r_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94AA8D9-7D3D-4114-970A-D1671B5A33B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456DBF9A-4C75-438E-AD28-93632393014E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F678959E-5C45-4896-80A4-1E09A95E6608}"/>
+    <workbookView xWindow="2355" yWindow="1950" windowWidth="23250" windowHeight="12570" xr2:uid="{F678959E-5C45-4896-80A4-1E09A95E6608}"/>
   </bookViews>
   <sheets>
     <sheet name="binek" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +499,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>